<commit_message>
user controltesting missing update
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leanne\Documents\sample_app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4035" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4035" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Model - testing" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
   <si>
     <t>Model</t>
   </si>
@@ -126,6 +131,12 @@
   </si>
   <si>
     <t>patients controller</t>
+  </si>
+  <si>
+    <t>destroy method is missing</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -155,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -174,6 +185,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -187,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -212,6 +229,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,15 +609,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -637,9 +657,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
user testdone, patients started
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Model</t>
   </si>
@@ -133,10 +133,13 @@
     <t>patients controller</t>
   </si>
   <si>
-    <t>destroy method is missing</t>
-  </si>
-  <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>admins_controller</t>
+  </si>
+  <si>
+    <t>destroy method is missing, update method does not work</t>
   </si>
 </sst>
 </file>
@@ -607,10 +610,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,19 +668,31 @@
         <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="D7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
testing of patient done, index file missing, admin controller testing commenced lots of bugs
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>destroy method is missing, update method does not work</t>
+  </si>
+  <si>
+    <t>you are missing the index view, so at this point in time all test which require an index fail. Good news this controller has a destroy method</t>
+  </si>
+  <si>
+    <t>:show</t>
+  </si>
+  <si>
+    <t>:index does not work (returns nil), :new does not work returns nil, :edit doesnt work (does not redirect and returns nil)</t>
+  </si>
+  <si>
+    <t>Leanne check :create again</t>
+  </si>
+  <si>
+    <t>:update remoces password, when no changes are suppose to occur</t>
   </si>
 </sst>
 </file>
@@ -610,10 +625,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +638,7 @@
     <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -640,27 +655,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -674,20 +689,40 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user, admin, doc and static ctl testing, static passed everything other need to be revised
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Model</t>
   </si>
@@ -139,9 +139,6 @@
     <t>admins_controller</t>
   </si>
   <si>
-    <t>destroy method is missing, update method does not work</t>
-  </si>
-  <si>
     <t>you are missing the index view, so at this point in time all test which require an index fail. Good news this controller has a destroy method</t>
   </si>
   <si>
@@ -151,10 +148,28 @@
     <t>:index does not work (returns nil), :new does not work returns nil, :edit doesnt work (does not redirect and returns nil)</t>
   </si>
   <si>
-    <t>Leanne check :create again</t>
-  </si>
-  <si>
-    <t>:update remoces password, when no changes are suppose to occur</t>
+    <t>:update remoces password, when it is sent into update, does not properly redirect to :edit</t>
+  </si>
+  <si>
+    <t>:delete method not found</t>
+  </si>
+  <si>
+    <t>:create does not increment or redirect</t>
+  </si>
+  <si>
+    <t>same as admin_controller, except also has undefined local variable or method patient_params</t>
+  </si>
+  <si>
+    <t>destroy method is missing, update method does not work, and the:show method does render the appropriate template</t>
+  </si>
+  <si>
+    <t>i dont know how to test this, what exactly is it doing in a backend context so i can check its occuring</t>
+  </si>
+  <si>
+    <t>no-read comment</t>
+  </si>
+  <si>
+    <t>need to test content of tthe views</t>
   </si>
 </sst>
 </file>
@@ -625,10 +640,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,14 +670,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="B2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>12</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,12 +700,24 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -686,7 +728,7 @@
         <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -700,7 +742,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -711,17 +753,25 @@
         <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="4" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
patient views rendering test all fails
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4035" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="4035" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model - testing" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>Model</t>
   </si>
@@ -170,6 +170,30 @@
   </si>
   <si>
     <t>need to test content of tthe views</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>_form</t>
+  </si>
+  <si>
+    <t>undefined method name when rendering this page</t>
+  </si>
+  <si>
+    <t>Content of the page not tested, only rending</t>
+  </si>
+  <si>
+    <t>first argument in fomr cannot contain or nill or be empty this might help http://stackoverflow.com/questions/17635634/first-argument-in-form-cannot-contain-nil-or-be-empty-comments</t>
   </si>
 </sst>
 </file>
@@ -237,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -267,6 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -783,149 +808,219 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C14" t="s">
-        <v>32</v>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all view render tested 50% pass
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -17,6 +17,7 @@
     <sheet name="html" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="76">
   <si>
     <t>Model</t>
   </si>
@@ -194,6 +195,66 @@
   </si>
   <si>
     <t>first argument in fomr cannot contain or nill or be empty this might help http://stackoverflow.com/questions/17635634/first-argument-in-form-cannot-contain-nil-or-be-empty-comments</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>undefined method each for nil class</t>
+  </si>
+  <si>
+    <t>Admins</t>
+  </si>
+  <si>
+    <t>layouts</t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>header</t>
+  </si>
+  <si>
+    <t>shim</t>
+  </si>
+  <si>
+    <t>templates renders</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>actionview:template:error (error on line7)</t>
+  </si>
+  <si>
+    <t>actionview:template:error (error on line7), this could be on my end but i dont think so but if you look at at and find im wrong let me know</t>
+  </si>
+  <si>
+    <t>sessions</t>
+  </si>
+  <si>
+    <t>newSpec</t>
+  </si>
+  <si>
+    <t>shared</t>
+  </si>
+  <si>
+    <t>errorSpec</t>
+  </si>
+  <si>
+    <t>Static_pages</t>
+  </si>
+  <si>
+    <t>about</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>home</t>
   </si>
 </sst>
 </file>
@@ -808,10 +869,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +1022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>50</v>
       </c>
@@ -975,7 +1036,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>49</v>
       </c>
@@ -992,7 +1053,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>51</v>
       </c>
@@ -1009,7 +1070,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
         <v>52</v>
       </c>
@@ -1021,6 +1082,326 @@
       </c>
       <c r="I20" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" t="s">
+        <v>35</v>
+      </c>
+      <c r="I31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" t="s">
+        <v>35</v>
+      </c>
+      <c r="I32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
+      </c>
+      <c r="H42" t="s">
+        <v>32</v>
+      </c>
+      <c r="I42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" t="s">
+        <v>32</v>
+      </c>
+      <c r="I45" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Pools to the application
</commit_message>
<xml_diff>
--- a/TestingLog.xlsx
+++ b/TestingLog.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leanne\Documents\sample_app\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9585" windowHeight="4035" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9585" windowHeight="4035" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model - testing" sheetId="1" r:id="rId1"/>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="83">
   <si>
     <t>Model</t>
   </si>
@@ -260,6 +255,21 @@
   </si>
   <si>
     <t>templates renders, has a routting error</t>
+  </si>
+  <si>
+    <t>Pool controller</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>Pools</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>should test that this does not have a render</t>
   </si>
 </sst>
 </file>
@@ -640,7 +650,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -648,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,6 +743,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -741,10 +756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,6 +891,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -884,10 +904,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,6 +1462,39 @@
         <v>63</v>
       </c>
     </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I52" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>